<commit_message>
joined attr to shape file and images
</commit_message>
<xml_diff>
--- a/matrix/Workbook2.xlsx
+++ b/matrix/Workbook2.xlsx
@@ -16,6 +16,7 @@
     <definedName name="vulnerability" localSheetId="1">V!$A$1:$R$193</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +28,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="readiness.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:brunosan:Projects:maps:matrix:resources:readiness:readiness.csv" thousands="_x0000_" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:brunosan:Projects:maps:matrix:resources:readiness:readiness.csv" comma="1">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -51,7 +52,7 @@
     </textPr>
   </connection>
   <connection id="2" name="vulnerability.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:brunosan:Projects:maps:matrix:resources:vulnerability:vulnerability.csv" thousands="_x0000_" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:brunosan:Projects:maps:matrix:resources:vulnerability:vulnerability.csv" tab="0" comma="1">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="394">
   <si>
     <t>ISO3</t>
   </si>
@@ -1257,6 +1258,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>limit</t>
   </si>
 </sst>
 </file>
@@ -1305,8 +1309,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1315,11 +1323,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -23325,7 +23337,7 @@
   <dimension ref="A1:J193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23357,7 +23369,7 @@
       </c>
       <c r="C2">
         <f>IF(V!R2&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="e">
         <f>B2+C2</f>
@@ -23425,11 +23437,11 @@
       </c>
       <c r="C6">
         <f>IF(V!R6&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -23442,7 +23454,7 @@
       </c>
       <c r="C7">
         <f>IF(V!R7&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="e">
         <f t="shared" si="0"/>
@@ -23465,6 +23477,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="H8" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
@@ -23521,7 +23536,7 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -23562,7 +23577,7 @@
       </c>
       <c r="H12">
         <f>I9+J10</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -23575,18 +23590,18 @@
       </c>
       <c r="C13">
         <f>IF(V!R13&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
         <v>389</v>
       </c>
       <c r="H13">
         <f>J9+J10</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -23599,11 +23614,11 @@
       </c>
       <c r="C14">
         <f>IF(V!R14&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
         <v>390</v>
@@ -23623,11 +23638,11 @@
       </c>
       <c r="C15">
         <f>IF(V!R15&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
         <v>391</v>
@@ -23698,11 +23713,11 @@
       </c>
       <c r="C19">
         <f>IF(V!R19&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -23715,11 +23730,11 @@
       </c>
       <c r="C20">
         <f>IF(V!R20&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -23732,11 +23747,11 @@
       </c>
       <c r="C21">
         <f>IF(V!R21&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -23749,11 +23764,11 @@
       </c>
       <c r="C22">
         <f>IF(V!R22&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -23783,11 +23798,11 @@
       </c>
       <c r="C24">
         <f>IF(V!R24&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -23851,11 +23866,11 @@
       </c>
       <c r="C28">
         <f>IF(V!R28&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -23868,11 +23883,11 @@
       </c>
       <c r="C29">
         <f>IF(V!R29&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -23885,11 +23900,11 @@
       </c>
       <c r="C30">
         <f>IF(V!R30&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -23902,11 +23917,11 @@
       </c>
       <c r="C31">
         <f>IF(V!R31&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -23953,11 +23968,11 @@
       </c>
       <c r="C34">
         <f>IF(V!R34&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -23970,11 +23985,11 @@
       </c>
       <c r="C35">
         <f>IF(V!R35&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -24038,11 +24053,11 @@
       </c>
       <c r="C39">
         <f>IF(V!R39&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -24055,11 +24070,11 @@
       </c>
       <c r="C40">
         <f>IF(V!R40&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -24089,11 +24104,11 @@
       </c>
       <c r="C42">
         <f>IF(V!R42&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -24106,11 +24121,11 @@
       </c>
       <c r="C43">
         <f>IF(V!R43&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -24208,11 +24223,11 @@
       </c>
       <c r="C49">
         <f>IF(V!R49&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -24225,11 +24240,11 @@
       </c>
       <c r="C50">
         <f>IF(V!R50&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -24310,11 +24325,11 @@
       </c>
       <c r="C55">
         <f>IF(V!R55&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -24327,11 +24342,11 @@
       </c>
       <c r="C56">
         <f>IF(V!R56&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -24361,11 +24376,11 @@
       </c>
       <c r="C58">
         <f>IF(V!R58&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -24378,11 +24393,11 @@
       </c>
       <c r="C59">
         <f>IF(V!R59&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -24429,11 +24444,11 @@
       </c>
       <c r="C62">
         <f>IF(V!R62&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -24446,11 +24461,11 @@
       </c>
       <c r="C63">
         <f>IF(V!R63&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -24497,11 +24512,11 @@
       </c>
       <c r="C66">
         <f>IF(V!R66&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -24531,7 +24546,7 @@
       </c>
       <c r="C68">
         <f>IF(V!R68&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D68" t="e">
         <f t="shared" si="1"/>
@@ -24548,11 +24563,11 @@
       </c>
       <c r="C69">
         <f>IF(V!R69&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D69">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -24565,11 +24580,11 @@
       </c>
       <c r="C70">
         <f>IF(V!R70&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D70">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -24582,11 +24597,11 @@
       </c>
       <c r="C71">
         <f>IF(V!R71&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D71">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -24599,11 +24614,11 @@
       </c>
       <c r="C72">
         <f>IF(V!R72&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -24616,7 +24631,7 @@
       </c>
       <c r="C73">
         <f>IF(V!R73&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D73" t="e">
         <f t="shared" si="1"/>
@@ -24633,11 +24648,11 @@
       </c>
       <c r="C74">
         <f>IF(V!R74&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -24684,11 +24699,11 @@
       </c>
       <c r="C77">
         <f>IF(V!R77&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D77">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -24735,7 +24750,7 @@
       </c>
       <c r="C80">
         <f>IF(V!R80&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D80" t="e">
         <f t="shared" si="1"/>
@@ -24803,11 +24818,11 @@
       </c>
       <c r="C84">
         <f>IF(V!R84&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -24871,11 +24886,11 @@
       </c>
       <c r="C88">
         <f>IF(V!R88&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D88">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -24888,7 +24903,7 @@
       </c>
       <c r="C89">
         <f>IF(V!R89&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D89" t="e">
         <f t="shared" si="1"/>
@@ -24905,7 +24920,7 @@
       </c>
       <c r="C90">
         <f>IF(V!R90&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D90" t="e">
         <f t="shared" si="1"/>
@@ -24973,11 +24988,11 @@
       </c>
       <c r="C94">
         <f>IF(V!R94&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D94">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -25024,11 +25039,11 @@
       </c>
       <c r="C97">
         <f>IF(V!R97&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D97">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -25041,11 +25056,11 @@
       </c>
       <c r="C98">
         <f>IF(V!R98&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D98">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -25126,11 +25141,11 @@
       </c>
       <c r="C103">
         <f>IF(V!R103&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D103">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -25143,11 +25158,11 @@
       </c>
       <c r="C104">
         <f>IF(V!R104&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D104">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -25177,7 +25192,7 @@
       </c>
       <c r="C106">
         <f>IF(V!R106&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D106" t="e">
         <f t="shared" si="1"/>
@@ -25194,11 +25209,11 @@
       </c>
       <c r="C107">
         <f>IF(V!R107&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D107">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -25228,7 +25243,7 @@
       </c>
       <c r="C109">
         <f>IF(V!R109&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D109" t="e">
         <f t="shared" si="1"/>
@@ -25245,11 +25260,11 @@
       </c>
       <c r="C110">
         <f>IF(V!R110&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D110">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -25296,7 +25311,7 @@
       </c>
       <c r="C113">
         <f>IF(V!R113&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D113" t="e">
         <f t="shared" si="1"/>
@@ -25364,11 +25379,11 @@
       </c>
       <c r="C117">
         <f>IF(V!R117&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D117">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -25398,11 +25413,11 @@
       </c>
       <c r="C119">
         <f>IF(V!R119&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D119">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -25415,11 +25430,11 @@
       </c>
       <c r="C120">
         <f>IF(V!R120&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D120">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -25432,11 +25447,11 @@
       </c>
       <c r="C121">
         <f>IF(V!R121&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D121">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -25449,11 +25464,11 @@
       </c>
       <c r="C122">
         <f>IF(V!R122&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D122">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -25483,11 +25498,11 @@
       </c>
       <c r="C124">
         <f>IF(V!R124&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D124">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -25551,11 +25566,11 @@
       </c>
       <c r="C128">
         <f>IF(V!R128&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D128">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -25568,11 +25583,11 @@
       </c>
       <c r="C129">
         <f>IF(V!R129&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D129">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -25619,11 +25634,11 @@
       </c>
       <c r="C132">
         <f>IF(V!R132&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D132">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -25636,7 +25651,7 @@
       </c>
       <c r="C133">
         <f>IF(V!R133&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D133" t="e">
         <f t="shared" si="2"/>
@@ -25653,11 +25668,11 @@
       </c>
       <c r="C134">
         <f>IF(V!R134&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D134">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -25670,11 +25685,11 @@
       </c>
       <c r="C135">
         <f>IF(V!R135&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D135">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -25704,11 +25719,11 @@
       </c>
       <c r="C137">
         <f>IF(V!R137&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D137">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -25823,11 +25838,11 @@
       </c>
       <c r="C144">
         <f>IF(V!R144&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D144">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -25840,7 +25855,7 @@
       </c>
       <c r="C145">
         <f>IF(V!R145&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D145" t="e">
         <f t="shared" si="2"/>
@@ -25857,11 +25872,11 @@
       </c>
       <c r="C146">
         <f>IF(V!R146&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D146">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -25874,7 +25889,7 @@
       </c>
       <c r="C147">
         <f>IF(V!R147&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D147" t="e">
         <f t="shared" si="2"/>
@@ -25891,11 +25906,11 @@
       </c>
       <c r="C148">
         <f>IF(V!R148&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D148">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -25925,11 +25940,11 @@
       </c>
       <c r="C150">
         <f>IF(V!R150&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D150">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -25959,11 +25974,11 @@
       </c>
       <c r="C152">
         <f>IF(V!R152&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D152">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -25993,7 +26008,7 @@
       </c>
       <c r="C154">
         <f>IF(V!R154&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D154" t="e">
         <f t="shared" si="2"/>
@@ -26010,11 +26025,11 @@
       </c>
       <c r="C155">
         <f>IF(V!R155&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D155">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -26078,7 +26093,7 @@
       </c>
       <c r="C159">
         <f>IF(V!R159&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D159" t="e">
         <f t="shared" si="2"/>
@@ -26095,7 +26110,7 @@
       </c>
       <c r="C160">
         <f>IF(V!R160&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D160" t="e">
         <f t="shared" si="2"/>
@@ -26112,11 +26127,11 @@
       </c>
       <c r="C161">
         <f>IF(V!R161&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D161">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -26163,7 +26178,7 @@
       </c>
       <c r="C164">
         <f>IF(V!R164&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D164" t="e">
         <f t="shared" si="2"/>
@@ -26197,11 +26212,11 @@
       </c>
       <c r="C166">
         <f>IF(V!R166&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D166">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -26265,11 +26280,11 @@
       </c>
       <c r="C170">
         <f>IF(V!R170&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D170">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -26282,11 +26297,11 @@
       </c>
       <c r="C171">
         <f>IF(V!R171&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D171">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -26316,7 +26331,7 @@
       </c>
       <c r="C173">
         <f>IF(V!R173&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D173" t="e">
         <f t="shared" si="2"/>
@@ -26333,11 +26348,11 @@
       </c>
       <c r="C174">
         <f>IF(V!R174&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D174">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -26350,11 +26365,11 @@
       </c>
       <c r="C175">
         <f>IF(V!R175&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D175">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -26367,11 +26382,11 @@
       </c>
       <c r="C176">
         <f>IF(V!R176&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D176">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -26435,7 +26450,7 @@
       </c>
       <c r="C180">
         <f>IF(V!R180&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D180" t="e">
         <f t="shared" si="2"/>
@@ -26452,11 +26467,11 @@
       </c>
       <c r="C181">
         <f>IF(V!R181&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D181">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -26571,11 +26586,11 @@
       </c>
       <c r="C188">
         <f>IF(V!R188&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D188">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -26622,11 +26637,11 @@
       </c>
       <c r="C191">
         <f>IF(V!R191&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D191">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -26639,11 +26654,11 @@
       </c>
       <c r="C192">
         <f>IF(V!R192&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D192">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -26656,11 +26671,11 @@
       </c>
       <c r="C193">
         <f>IF(V!R193&lt;Matrix!$H$10,Matrix!$I$10,Matrix!$J$10)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D193">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>